<commit_message>
Need to calculate more metrics. csv update
</commit_message>
<xml_diff>
--- a/detection_metrics.xlsx
+++ b/detection_metrics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t xml:space="preserve">Filename</t>
   </si>
@@ -70,13 +70,31 @@
     <t xml:space="preserve">pc19.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Actual 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">pc20.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Observed 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training</t>
+  </si>
+  <si>
     <t xml:space="preserve">pc21.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Verication</t>
+  </si>
+  <si>
     <t xml:space="preserve">pc22.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observed 0</t>
   </si>
   <si>
     <t xml:space="preserve">pc23.png</t>
@@ -314,10 +332,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,10 +567,16 @@
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.88</v>
@@ -569,10 +593,16 @@
       <c r="F12" s="0" t="n">
         <v>16.01</v>
       </c>
+      <c r="H12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.95</v>
@@ -589,10 +619,13 @@
       <c r="F13" s="0" t="n">
         <v>13.1</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.09</v>
@@ -609,10 +642,16 @@
       <c r="F14" s="0" t="n">
         <v>7.14</v>
       </c>
+      <c r="H14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.94</v>
@@ -629,10 +668,13 @@
       <c r="F15" s="0" t="n">
         <v>17.33</v>
       </c>
+      <c r="I15" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.86</v>
@@ -652,7 +694,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.54</v>
@@ -672,7 +714,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.42</v>
@@ -692,7 +734,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.62</v>
@@ -712,7 +754,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -732,7 +774,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -752,7 +794,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">AVERAGE(B2:B21)</f>
@@ -777,7 +819,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">STDEV(B2:B21)</f>

</xml_diff>